<commit_message>
Added Hands On Demos - Day 1.
</commit_message>
<xml_diff>
--- a/Setup and Installation/Required Software and Setup.xlsx
+++ b/Setup and Installation/Required Software and Setup.xlsx
@@ -103,10 +103,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -157,7 +157,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -171,6 +178,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -179,106 +224,61 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,187 +302,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,6 +493,63 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -507,15 +564,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -537,54 +585,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -596,15 +596,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -617,127 +617,127 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1101,14 +1101,14 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19:C20"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="$A13:$XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="38.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="76.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="77.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Hands On Demos - Day 6.
</commit_message>
<xml_diff>
--- a/Setup and Installation/Required Software and Setup.xlsx
+++ b/Setup and Installation/Required Software and Setup.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Serial No.</t>
   </si>
@@ -97,16 +97,28 @@
   <si>
     <t>https://dev.mysql.com/downloads/mysql/</t>
   </si>
+  <si>
+    <t>Git Download for Windows</t>
+  </si>
+  <si>
+    <t>https://git-scm.com/download/win</t>
+  </si>
+  <si>
+    <t>GitHub account</t>
+  </si>
+  <si>
+    <t>https://github.com/join</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -156,6 +168,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -163,8 +213,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,21 +230,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -224,23 +260,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,37 +291,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,25 +314,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,157 +494,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,11 +508,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -508,8 +526,34 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -529,41 +573,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,18 +599,16 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -617,127 +629,127 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -771,9 +783,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1101,7 +1111,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="$A13:$XFD13"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="$A15:$XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1213,15 +1223,30 @@
     <row r="14" spans="1:1">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="7"/>
+    <row r="15" ht="18.75" spans="1:3">
+      <c r="A15" s="7">
+        <v>7</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="7"/>
     </row>
-    <row r="17" ht="18.75" spans="1:2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="13"/>
+    <row r="17" ht="18.75" spans="1:3">
+      <c r="A17" s="7">
+        <v>8</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="19" ht="18.75" spans="1:2">
       <c r="A19" s="7"/>
@@ -1249,6 +1274,8 @@
     <hyperlink ref="C9" r:id="rId4" display="https://maven.apache.org/download.cgi"/>
     <hyperlink ref="C11" r:id="rId5" display="https://tomcat.apache.org/download-90.cgi"/>
     <hyperlink ref="C13" r:id="rId6" display="https://dev.mysql.com/downloads/mysql/"/>
+    <hyperlink ref="C15" r:id="rId7" display="https://git-scm.com/download/win"/>
+    <hyperlink ref="C17" r:id="rId8" display="https://github.com/join"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>